<commit_message>
Changed format of import excel sheet to match data display on site
</commit_message>
<xml_diff>
--- a/infrastructureinventoryproject/infrastructureinventoryapp/static/FormatSample.xlsx
+++ b/infrastructureinventoryproject/infrastructureinventoryapp/static/FormatSample.xlsx
@@ -81,15 +81,6 @@
     <t>Purchase Order</t>
   </si>
   <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>Next Hardware Support Date</t>
-  </si>
-  <si>
-    <t>Base Warranty</t>
-  </si>
-  <si>
     <t>CPU</t>
   </si>
   <si>
@@ -114,12 +105,6 @@
     <t>Primary Application</t>
   </si>
   <si>
-    <t>Is Virtual Machine</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -139,6 +124,21 @@
   </si>
   <si>
     <t>Network</t>
+  </si>
+  <si>
+    <t>Is Virtual Machine (TRUE / FALSE)</t>
+  </si>
+  <si>
+    <t>Environment (Prod / Dev / QA)</t>
+  </si>
+  <si>
+    <t>Start Date (MM/DD/YY)</t>
+  </si>
+  <si>
+    <t>Next Hardware Support Date (MM/DD/YY)</t>
+  </si>
+  <si>
+    <t>Base Warranty (MM/DD/YY)</t>
   </si>
 </sst>
 </file>
@@ -520,15 +520,15 @@
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
     <col min="9" max="9" width="26.5" customWidth="1"/>
     <col min="10" max="10" width="16.83203125" customWidth="1"/>
@@ -542,46 +542,46 @@
     <col min="20" max="20" width="16.6640625" customWidth="1"/>
     <col min="21" max="21" width="21.5" customWidth="1"/>
     <col min="22" max="22" width="21" customWidth="1"/>
-    <col min="23" max="23" width="31.1640625" customWidth="1"/>
-    <col min="24" max="24" width="17.6640625" customWidth="1"/>
+    <col min="23" max="23" width="37.33203125" customWidth="1"/>
+    <col min="24" max="24" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>11</v>
@@ -611,28 +611,28 @@
         <v>19</v>
       </c>
       <c r="V1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:29">

</xml_diff>

<commit_message>
Displaying All Fields except notes in tables, including notes in import
Now, all fields display on the home page and the import confirmation page. When importing from excel, Notes are now possible to import as well in the last column of the sheet. The sample sheet has been updated accordingly
</commit_message>
<xml_diff>
--- a/infrastructureinventoryproject/infrastructureinventoryapp/static/FormatSample.xlsx
+++ b/infrastructureinventoryproject/infrastructureinventoryapp/static/FormatSample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve"> Signiant Agent</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Base Warranty (MM/DD/YY)</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -517,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -546,7 +549,7 @@
     <col min="24" max="24" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="2" customFormat="1">
+    <row r="1" spans="1:30" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -634,8 +637,11 @@
       <c r="AC1" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="AD1" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>0</v>
       </c>

</xml_diff>